<commit_message>
created csat datasets, added to csat cleaning script
</commit_message>
<xml_diff>
--- a/Gage_stats.xlsx
+++ b/Gage_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\DRAFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72B47B-061F-4935-81C0-5D18C5334F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9F5E5B-E111-434C-9B0C-5D2C82D1929B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="20" windowWidth="19380" windowHeight="20950" xr2:uid="{D4700E98-1309-4C30-9B7A-3AB0B7666C33}"/>
+    <workbookView xWindow="-110" yWindow="-90" windowWidth="38620" windowHeight="21080" xr2:uid="{D4700E98-1309-4C30-9B7A-3AB0B7666C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="66">
   <si>
     <t>Gage</t>
   </si>
@@ -186,6 +186,54 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>COPI2</t>
+  </si>
+  <si>
+    <t>IL03</t>
+  </si>
+  <si>
+    <t>IL04</t>
+  </si>
+  <si>
+    <t>IL05</t>
+  </si>
+  <si>
+    <t>IL06</t>
+  </si>
+  <si>
+    <t>IL07</t>
+  </si>
+  <si>
+    <t>IL08</t>
+  </si>
+  <si>
+    <t>LSLI2</t>
+  </si>
+  <si>
+    <t>Marseilles</t>
+  </si>
+  <si>
+    <t>Dresden</t>
+  </si>
+  <si>
+    <t>Starved Rock</t>
+  </si>
+  <si>
+    <t>Peoria</t>
+  </si>
+  <si>
+    <t>LaGrange</t>
   </si>
 </sst>
 </file>
@@ -267,9 +315,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +355,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -413,7 +461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -563,18 +611,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8EC03F-55CA-4AAE-B75D-F40E88D76768}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,8 +642,23 @@
       <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -616,8 +680,23 @@
       <c r="G2" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1">
+        <v>419.9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -636,8 +715,23 @@
       <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="1">
+        <v>511.45</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -656,8 +750,23 @@
       <c r="F4" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1">
+        <v>563.21</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -676,8 +785,23 @@
       <c r="F5" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -696,8 +820,23 @@
       <c r="F6" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="1">
+        <v>585.47</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,8 +855,23 @@
       <c r="F7" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="1">
+        <v>535.16</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -736,8 +890,23 @@
       <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="1">
+        <v>472.71</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -759,8 +928,23 @@
       <c r="G9" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -779,8 +963,23 @@
       <c r="F10" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="1">
+        <v>449.43</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -799,8 +998,23 @@
       <c r="F11" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="2">
+        <v>447.42</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -819,8 +1033,26 @@
       <c r="F12" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -839,8 +1071,26 @@
       <c r="F13" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -859,8 +1109,26 @@
       <c r="F14" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -879,8 +1147,26 @@
       <c r="F15" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -902,8 +1188,23 @@
       <c r="G16" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -925,8 +1226,23 @@
       <c r="G17" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -945,8 +1261,26 @@
       <c r="F18" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -965,8 +1299,26 @@
       <c r="F19" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -985,8 +1337,26 @@
       <c r="F20" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1005,8 +1375,26 @@
       <c r="F21" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1025,8 +1413,26 @@
       <c r="F22" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J22" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1045,8 +1451,26 @@
       <c r="F23" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J23" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -1065,8 +1489,23 @@
       <c r="F24" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1085,8 +1524,23 @@
       <c r="F25" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1105,8 +1559,23 @@
       <c r="F26" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1125,8 +1594,23 @@
       <c r="F27" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -1145,8 +1629,23 @@
       <c r="F28" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
@@ -1165,8 +1664,23 @@
       <c r="F29" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -1185,8 +1699,23 @@
       <c r="F30" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -1205,8 +1734,23 @@
       <c r="F31" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
@@ -1225,8 +1769,23 @@
       <c r="F32" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -1245,8 +1804,23 @@
       <c r="F33" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
@@ -1265,8 +1839,23 @@
       <c r="F34" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -1285,8 +1874,23 @@
       <c r="F35" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1305,8 +1909,23 @@
       <c r="F36" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
@@ -1325,8 +1944,23 @@
       <c r="F37" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
@@ -1345,8 +1979,23 @@
       <c r="F38" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -1365,8 +2014,23 @@
       <c r="F39" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1385,8 +2049,23 @@
       <c r="F40" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -1405,8 +2084,23 @@
       <c r="F41" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
@@ -1425,8 +2119,23 @@
       <c r="F42" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1445,8 +2154,23 @@
       <c r="F43" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -1465,8 +2189,23 @@
       <c r="F44" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -1485,8 +2224,23 @@
       <c r="F45" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>30</v>
       </c>
@@ -1505,8 +2259,23 @@
       <c r="F46" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -1523,6 +2292,140 @@
         <v>43</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="K48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K53" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="11:15" x14ac:dyDescent="0.35">
+      <c r="K54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O54" s="1" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>